<commit_message>
finished username & email Checker in real time
</commit_message>
<xml_diff>
--- a/doc/logBook/logBookBFA.xlsx
+++ b/doc/logBook/logBookBFA.xlsx
@@ -541,7 +541,7 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,10 +953,15 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
+      <c r="B23" s="6">
+        <v>44277</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0.3347222222222222</v>
+      </c>
       <c r="E23" s="2">
         <f>Tableau2[[#This Row],[Heure de fin]]-Tableau2[[#This Row],[Heure de début]]</f>
-        <v>0</v>
+        <v>-0.3347222222222222</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1434,7 +1439,7 @@
     <row r="101" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E101" s="10">
         <f>SUM(Tableau2[Temps])</f>
-        <v>1.4201388888888893</v>
+        <v>1.0854166666666671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>